<commit_message>
minor fixes and reporting enhancements
1. ExcelFileManager: reformat returned numeric values to remove .0 in
case of round numbers.
2. FileManager: created copyFolder, zipFiles
3. ReportManager: created generateAllureReportArchive,
populateEnvironmentData
4. SSHActions: created executeShellCommand
5. create/open_allure_report.sh: bundled some commands to bash files to
ease report generation and manipulation.
6. pom.xml: added flag to automaticallyGenerateAllureReport
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/testSuite01/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/testSuite01/TestData.xlsx
@@ -65,7 +65,7 @@
     <t xml:space="preserve">Search Query</t>
   </si>
   <si>
-    <t xml:space="preserve">Selenium</t>
+    <t xml:space="preserve">Search Query 2</t>
   </si>
   <si>
     <t xml:space="preserve">Supported Browser Types</t>
@@ -291,10 +291,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -366,12 +366,20 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>14</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>12.2</v>
       </c>
     </row>
   </sheetData>
@@ -409,7 +417,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.53"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
version bump to 2.0 after linting, minor fixes for sample test classes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/testSuite01/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/testSuite01/TestData.xlsx
@@ -26,13 +26,13 @@
     <t xml:space="preserve">Variable</t>
   </si>
   <si>
-    <t xml:space="preserve">Value 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value 3</t>
+    <t xml:space="preserve">Data1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data3</t>
   </si>
   <si>
     <t xml:space="preserve">Settings</t>
@@ -294,7 +294,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
adding unit test cases and fixing issues
. BrowserActions: implemented fix for issue with window maximization
. ElementActions: reorganizing, creating waitForElementToBePresent,
deprecating canFindUniqueElementForInternalUse(WebDriver driver, By
elementLocator, int timeout)
. ExcelFileManager: restyling, fixing issue with empty rows throwing an
exception.
. pom.xml: version bump
. ReportManager: minor change to exception text
. ScreenshotManager: restyling, switching from
internalCanFindUniqueElement to getElementsCount.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/testSuite01/TestData.xlsx
+++ b/src/test/resources/TestDataFiles/testSuite01/TestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t xml:space="preserve">Search Query 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testRowValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testRowData.</t>
   </si>
   <si>
     <t xml:space="preserve">Supported Browser Types</t>
@@ -291,10 +297,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -380,6 +386,14 @@
       </c>
       <c r="B9" s="0" t="n">
         <v>12.2</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -423,12 +437,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -438,12 +452,12 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>